<commit_message>
failing project page during deployment
</commit_message>
<xml_diff>
--- a/content/content.xlsx
+++ b/content/content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\brej-portfolio\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDB777A-AD3B-42A6-BD05-F5CADF305F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D509FF0D-2B65-4A62-BD11-B470D8387CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="152">
   <si>
     <t>Portfolio content.xlsx template (for scripts/generate-content.mjs)</t>
   </si>
@@ -476,13 +476,25 @@
   </si>
   <si>
     <t>brejesh.bala@gmail.com</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-30</t>
+  </si>
+  <si>
+    <t>2025-13</t>
+  </si>
+  <si>
+    <t>testing-essay-writer</t>
+  </si>
+  <si>
+    <t>ABC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,6 +517,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1131,7 +1149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1684,11 +1702,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1774,7 +1792,43 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" t="s">
+        <v>149</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
pre final changes dones
</commit_message>
<xml_diff>
--- a/content/content.xlsx
+++ b/content/content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\brej-portfolio\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF18ED3-F7E9-49E5-BEB4-48F5D284EF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C8A4EA-2D67-4B69-8CFB-713C98F5B484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="428">
   <si>
     <t>Portfolio content.xlsx template (for scripts/generate-content.mjs)</t>
   </si>
@@ -238,15 +238,6 @@
     <t>liveUrl</t>
   </si>
   <si>
-    <t>Essay Writer App</t>
-  </si>
-  <si>
-    <t>Streamlit app that generates structured essays with export options.</t>
-  </si>
-  <si>
-    <t>Streamlit;LLM;NLP</t>
-  </si>
-  <si>
     <t>Python;Streamlit;LangChain</t>
   </si>
   <si>
@@ -277,15 +268,6 @@
     <t>proj-essay-writer</t>
   </si>
   <si>
-    <t>Generate structured essays with export.</t>
-  </si>
-  <si>
-    <t>A Streamlit app that helps users generate structured essays with consistent sections and export options.</t>
-  </si>
-  <si>
-    <t>Clean UI workflow;Export options;Prompt tuning</t>
-  </si>
-  <si>
     <t>2025-12</t>
   </si>
   <si>
@@ -415,18 +397,6 @@
     <t>brejesh.bala@gmail.com</t>
   </si>
   <si>
-    <t>https://github.com/brej-30</t>
-  </si>
-  <si>
-    <t>2025-13</t>
-  </si>
-  <si>
-    <t>testing-essay-writer</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
     <t>Data Scientist / ML Engineer → End-to-End ML (Train → Deploy) | Production-Ready Portfolio</t>
   </si>
   <si>
@@ -914,6 +884,438 @@
   </si>
   <si>
     <t>Digital Marketing;Outreach;Communication</t>
+  </si>
+  <si>
+    <t>proj-dogbreed-classification</t>
+  </si>
+  <si>
+    <t>Dog Breed Classification</t>
+  </si>
+  <si>
+    <t>Deep learning pipeline for 120-breed classification with transfer learning.</t>
+  </si>
+  <si>
+    <t>End-to-end deep learning solution leveraging MobileNetV2 transfer learning to classify 120 dog breeds with optimized accuracy. Demonstrates proficiency in computer vision, data preprocessing, and model architecture selection—key skills for ML production environments.</t>
+  </si>
+  <si>
+    <t>TensorFlow;Transfer Learning;CNN;Computer Vision</t>
+  </si>
+  <si>
+    <t>Python;TensorFlow;Jupyter</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/Logicmojo-AIML-Assignments-DogBreedClassificationTensorFlow</t>
+  </si>
+  <si>
+    <t>Transfer learning optimization;120-class multi-label classification;Production-ready preprocessing pipeline</t>
+  </si>
+  <si>
+    <t>proj-heart-disease</t>
+  </si>
+  <si>
+    <t>Heart Disease Risk Predictor</t>
+  </si>
+  <si>
+    <t>Predictive model for cardiac disease classification from medical data.</t>
+  </si>
+  <si>
+    <t>Comprehensive supervised learning pipeline for predicting heart disease risk using patient medical records. Features rigorous data exploration, model selection across multiple algorithms, hyperparameter tuning, and cross-validation—demonstrating systematic ML workflow and healthcare domain understanding.</t>
+  </si>
+  <si>
+    <t>Machine Learning;Classification;Healthcare Analytics;Feature Engineering</t>
+  </si>
+  <si>
+    <t>Python;Scikit-learn;Pandas;Numpy</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/Logicmojo-AIML-Assignments-heart-disease-prediction-ml</t>
+  </si>
+  <si>
+    <t>Multi-algorithm comparison;Cross-validated evaluation;Medical data preprocessing</t>
+  </si>
+  <si>
+    <t>proj-bulldozer-price</t>
+  </si>
+  <si>
+    <t>Heavy Equipment Price Prediction</t>
+  </si>
+  <si>
+    <t>Regression model for predicting equipment resale values.</t>
+  </si>
+  <si>
+    <t>Full-stack data science project predicting bulldozer auction prices using real-world commodity data. Covers complete pipeline: feature engineering, handling temporal data, model ensembling with XGBoost, and RMSLE optimization. Demonstrates end-to-end problem-solving from raw data to production predictions.</t>
+  </si>
+  <si>
+    <t>Regression;XGBoost;Ensemble Methods;Time-Series Features</t>
+  </si>
+  <si>
+    <t>Python;XGBoost;Scikit-learn;Pandas</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/Logicmojo-AIML-Assignments-bulldozer-price-prediction</t>
+  </si>
+  <si>
+    <t>XGBoost ensembling;Feature engineering for auction data;RMSLE optimization;Real-world dataset handling</t>
+  </si>
+  <si>
+    <t>2025-09</t>
+  </si>
+  <si>
+    <t>proj-otaku-oracle</t>
+  </si>
+  <si>
+    <t>Otaku Oracle</t>
+  </si>
+  <si>
+    <t>Intelligent anime recommendation engine powered by NLP.</t>
+  </si>
+  <si>
+    <t>AI-driven recommendation system applying NLP and collaborative filtering to anime datasets. Demonstrates understanding of recommendation systems, text processing, and user preference modeling—critical for personalization in production ML systems.</t>
+  </si>
+  <si>
+    <t>NLP;Recommendation Systems;Collaborative Filtering</t>
+  </si>
+  <si>
+    <t>Python;NLTK;Scikit-learn</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/otaku-oracle</t>
+  </si>
+  <si>
+    <t>Custom recommendation algorithm;NLP-based feature extraction;Cold-start problem handling</t>
+  </si>
+  <si>
+    <t>2025-08</t>
+  </si>
+  <si>
+    <t>proj-meal-planner</t>
+  </si>
+  <si>
+    <t>Daily Meal Planner</t>
+  </si>
+  <si>
+    <t>Personalized nutrition planning with Streamlit interface.</t>
+  </si>
+  <si>
+    <t>Interactive Streamlit application generating daily meal plans based on nutritional goals and dietary constraints. Showcases full-stack ML application development: requirement gathering, algorithm design, and user-centric UI/UX implementation.</t>
+  </si>
+  <si>
+    <t>Streamlit;Nutrition Algorithm;API Integration</t>
+  </si>
+  <si>
+    <t>Python;Streamlit;APIs</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/daily-meal-planner-streamlit</t>
+  </si>
+  <si>
+    <t>https://daily-meal-planner.streamlit.app/</t>
+  </si>
+  <si>
+    <t>Intelligent constraint solver;Real-time API data;Production Streamlit deployment</t>
+  </si>
+  <si>
+    <t>2025-07</t>
+  </si>
+  <si>
+    <t>proj-workout-planner</t>
+  </si>
+  <si>
+    <t>Daily Workout Planner</t>
+  </si>
+  <si>
+    <t>ML-powered fitness program generator.</t>
+  </si>
+  <si>
+    <t>Smart workout recommendation engine tailored to user fitness levels, goals, and equipment availability. Demonstrates machine learning application in domain-specific personalization and real-time system adaptability.</t>
+  </si>
+  <si>
+    <t>Streamlit;Fitness Algorithm;Personalization</t>
+  </si>
+  <si>
+    <t>Python;Streamlit;Pandas</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/daily-workout-planner</t>
+  </si>
+  <si>
+    <t>Progressive workout scaling;Goal-oriented recommendations;Equipment constraint handling</t>
+  </si>
+  <si>
+    <t>2025-06</t>
+  </si>
+  <si>
+    <t>proj-aurora-chat</t>
+  </si>
+  <si>
+    <t>Aurora Chat</t>
+  </si>
+  <si>
+    <t>Real-time AI chatbot with LLM integration.</t>
+  </si>
+  <si>
+    <t>Production-grade conversational AI application leveraging LLMs for natural dialogue. Demonstrates prompt engineering, context management, and real-time inference optimization—essential for modern ML applications in NLP.</t>
+  </si>
+  <si>
+    <t>LLM;NLP;Chatbot;Prompt Engineering</t>
+  </si>
+  <si>
+    <t>Python;Streamlit;LangChain;OpenAI API</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/aurora-chat-streamlit</t>
+  </si>
+  <si>
+    <t>https://aurora-chat.streamlit.app/</t>
+  </si>
+  <si>
+    <t>LLM prompt optimization;Token-efficient context handling;Real-time streaming responses</t>
+  </si>
+  <si>
+    <t>2025-05</t>
+  </si>
+  <si>
+    <t>proj-hr-analytics</t>
+  </si>
+  <si>
+    <t>HR Analytics Dashboard</t>
+  </si>
+  <si>
+    <t>Workforce intelligence platform with Power BI.</t>
+  </si>
+  <si>
+    <t>Comprehensive business analytics dashboard analyzing HR metrics, employee performance, and organizational trends. Demonstrates data visualization expertise, business intelligence fundamentals, and ability to translate data insights into actionable business metrics.</t>
+  </si>
+  <si>
+    <t>Power BI;Business Analytics;Data Visualization;KPI Tracking</t>
+  </si>
+  <si>
+    <t>Power BI;SQL;Excel</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/hr-analytics-dashboard-powerbi</t>
+  </si>
+  <si>
+    <t>Interactive KPI dashboards;Employee retention analytics;Drill-down analytics</t>
+  </si>
+  <si>
+    <t>2025-04</t>
+  </si>
+  <si>
+    <t>Essay Writer</t>
+  </si>
+  <si>
+    <t>Intelligent essay generation with structured outputs.</t>
+  </si>
+  <si>
+    <t>LLM-powered content generation system producing well-structured essays with customizable prompts and export functionality. Demonstrates prompt tuning, output formatting, and practical application of language models for content generation.</t>
+  </si>
+  <si>
+    <t>LLM;NLP;Content Generation;Prompt Engineering</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/essay-writer-streamlit</t>
+  </si>
+  <si>
+    <t>Structured prompt templates;Multi-format export;Iterative refinement capability</t>
+  </si>
+  <si>
+    <t>2025-03</t>
+  </si>
+  <si>
+    <t>proj-disaster-nlp</t>
+  </si>
+  <si>
+    <t>Disaster Tweets NLP Benchmarks</t>
+  </si>
+  <si>
+    <t>Multi-model NLP comparison for tweet classification.</t>
+  </si>
+  <si>
+    <t>Comprehensive NLP project benchmarking multiple models for disaster-related tweet classification. Tests diverse architectures (LSTM, BERT, TF-IDF + ML) and demonstrates strong experimental rigor, model evaluation methodology, and understanding of NLP fundamentals.</t>
+  </si>
+  <si>
+    <t>NLP;Text Classification;Model Benchmarking;LSTM;Transformers</t>
+  </si>
+  <si>
+    <t>Python;TensorFlow;Scikit-learn;NLTK</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/disaster-tweets-nlp-model-benchmarks</t>
+  </si>
+  <si>
+    <t>Multi-model comparison framework;BERT fine-tuning;Imbalanced classification handling</t>
+  </si>
+  <si>
+    <t>2025-02</t>
+  </si>
+  <si>
+    <t>proj-inventory-classifier</t>
+  </si>
+  <si>
+    <t>Inventory Bin Count Classifier</t>
+  </si>
+  <si>
+    <t>AWS SageMaker production ML model for inventory quantification.</t>
+  </si>
+  <si>
+    <t>End-to-end ML solution deployed on AWS SageMaker for automated inventory bin counting from images. Demonstrates cloud ML platforms expertise, model deployment at scale, and MLOps fundamentals—critical for enterprise data science roles.</t>
+  </si>
+  <si>
+    <t>AWS SageMaker;Computer Vision;MLOps;Cloud Deployment</t>
+  </si>
+  <si>
+    <t>Python;AWS SageMaker;TensorFlow</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/inventory-bin-count-classifier-aws-sagemaker</t>
+  </si>
+  <si>
+    <t>SageMaker model deployment;Real-time inference API;Automated retraining pipeline</t>
+  </si>
+  <si>
+    <t>2025-01</t>
+  </si>
+  <si>
+    <t>proj-aws-ml-nanodegree</t>
+  </si>
+  <si>
+    <t>Comprehensive AWS ML engineering curriculum projects.</t>
+  </si>
+  <si>
+    <t>Complete Udacity nanodegree covering AWS ML services, MLOps, and production ML pipelines. Includes projects on SageMaker, model deployment, monitoring, and hyperparameter optimization—essential competencies for ML engineering roles.</t>
+  </si>
+  <si>
+    <t>AWS;MLOps;SageMaker;ML Pipeline</t>
+  </si>
+  <si>
+    <t>Python;AWS;Jupyter</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/udacity-AWS-ml-engineer-nanodegree</t>
+  </si>
+  <si>
+    <t>Hyperparameter optimization;Model monitoring;MLOps best practices;Automated pipelines</t>
+  </si>
+  <si>
+    <t>2024-12</t>
+  </si>
+  <si>
+    <t>proj-customer-churn</t>
+  </si>
+  <si>
+    <t>Customer Churn MLOps</t>
+  </si>
+  <si>
+    <t>Production ML system with MLOps implementation.</t>
+  </si>
+  <si>
+    <t>Enterprise-grade machine learning project implementing complete MLOps lifecycle: data pipelines, model versioning, monitoring, and continuous retraining. Predicts customer churn with focus on production reliability, scalability, and reproducibility—directly aligning with data science role requirements.</t>
+  </si>
+  <si>
+    <t>MLOps;Model Monitoring;Pipeline Automation;XGBoost</t>
+  </si>
+  <si>
+    <t>Python;XGBoost;MLflow;AWS</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/customer-churn-mlops</t>
+  </si>
+  <si>
+    <t>ML pipeline automation;Model versioning &amp; registry;Performance monitoring;Retraining workflows</t>
+  </si>
+  <si>
+    <t>2024-11</t>
+  </si>
+  <si>
+    <t>https://brejesh-daily-workout-planner.streamlit.app/</t>
+  </si>
+  <si>
+    <t>proj-stock-terminal</t>
+  </si>
+  <si>
+    <t>Stock Mini Terminal</t>
+  </si>
+  <si>
+    <t>Real-time stock analysis with fundamentals and technical indicators.</t>
+  </si>
+  <si>
+    <t>Production-grade financial analytics platform providing ticker search, price performance tracking, fundamental analysis, and news aggregation. Demonstrates proficiency in financial data processing, API integration, and building decision-support tools—valuable for data science roles in fintech and quantitative analysis.</t>
+  </si>
+  <si>
+    <t>Streamlit;Financial Analytics;API Integration;Data Visualization</t>
+  </si>
+  <si>
+    <t>Python;Streamlit;yfinance;APIs</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/stock-mini-terminal-streamlit</t>
+  </si>
+  <si>
+    <t>https://stock-terminal.streamlit.app/</t>
+  </si>
+  <si>
+    <t>Real-time market data;Multi-source aggregation;Technical indicators dashboard</t>
+  </si>
+  <si>
+    <t>proj-data-insights-portal</t>
+  </si>
+  <si>
+    <t>Collaborative Data Insights Portal</t>
+  </si>
+  <si>
+    <t>Multi-user analytics platform for team-based data exploration.</t>
+  </si>
+  <si>
+    <t>Enterprise-level collaborative analytics application enabling teams to share datasets, generate insights, and visualize findings collectively. Showcases understanding of multi-user systems, data governance, and collaborative workflows—critical for data science teams in production environments.</t>
+  </si>
+  <si>
+    <t>Streamlit;Collaboration;Data Analytics;Dashboard</t>
+  </si>
+  <si>
+    <t>Python;Streamlit;Pandas;Plotly</t>
+  </si>
+  <si>
+    <t>https://github.com/brej-29/collaborative-data-insights-portal</t>
+  </si>
+  <si>
+    <t>Multi-user architecture;Shared dataset management;Interactive visualization;Role-based workflows</t>
+  </si>
+  <si>
+    <t>Production ML system with end-to-end MLOps pipeline, model versioning, monitoring, and automated retraining—demonstrating enterprise-grade data science and ML engineering capabilities.</t>
+  </si>
+  <si>
+    <t>MLOps;Model Monitoring;XGBoost;Pipeline Automation</t>
+  </si>
+  <si>
+    <t>AWS SageMaker-deployed computer vision model for real-time inventory quantification, showcasing cloud ML infrastructure, production deployment, and scalable inference.</t>
+  </si>
+  <si>
+    <t>Python;AWS SageMaker;TensorFlow;Docker</t>
+  </si>
+  <si>
+    <t>Multi-model NLP comparison framework benchmarking LSTM, BERT, and traditional ML approaches for text classification—demonstrating rigorous ML experimentation and deep NLP expertise.</t>
+  </si>
+  <si>
+    <t>NLP;Text Classification;BERT;Model Benchmarking</t>
+  </si>
+  <si>
+    <t>Python;TensorFlow;PyTorch;Scikit-learn</t>
+  </si>
+  <si>
+    <t>Transfer learning pipeline leveraging MobileNetV2 to classify 120 dog breeds, demonstrating computer vision mastery and production-ready deep learning architecture.</t>
+  </si>
+  <si>
+    <t>Transfer Learning;CNN;Computer Vision;TensorFlow</t>
+  </si>
+  <si>
+    <t>Python;TensorFlow;Keras;Jupyter</t>
+  </si>
+  <si>
+    <t>End-to-end regression project predicting bulldozer auction prices with advanced feature engineering, XGBoost ensembling, and RMSLE optimization on real-world commodity data.</t>
+  </si>
+  <si>
+    <t>XGBoost;Regression;Feature Engineering;Ensemble Methods</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -997,6 +1399,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1363,9 +1766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1378,30 +1781,30 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1431,13 +1834,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>36</v>
@@ -1445,13 +1848,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1459,13 +1862,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C3" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1473,13 +1876,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1487,13 +1890,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B5" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C5" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -1501,13 +1904,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B6" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C6" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1515,13 +1918,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -1529,13 +1932,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B8" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C8" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -1543,13 +1946,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="C9" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -1557,13 +1960,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C10" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -1592,13 +1995,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>36</v>
@@ -1606,13 +2009,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1620,13 +2023,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1634,13 +2037,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1648,13 +2051,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -1662,13 +2065,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1698,33 +2101,33 @@
   <sheetData>
     <row r="1" spans="1:5" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C2" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="E2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1814,16 +2217,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F2" t="s">
         <v>27</v>
@@ -1838,19 +2241,19 @@
         <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="K2" t="s">
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="M2" t="s">
         <v>31</v>
       </c>
       <c r="N2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="O2" t="s">
         <v>32</v>
@@ -1941,7 +2344,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
@@ -1996,7 +2399,7 @@
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2021,7 +2424,7 @@
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -2035,7 +2438,7 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -2049,7 +2452,7 @@
         <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -2057,7 +2460,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
         <v>57</v>
@@ -2068,13 +2471,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -2082,13 +2485,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -2096,13 +2499,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -2110,10 +2513,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -2121,10 +2524,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D12">
         <v>11</v>
@@ -2132,10 +2535,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B13" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D13">
         <v>12</v>
@@ -2143,10 +2546,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D14">
         <v>13</v>
@@ -2154,13 +2557,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D15">
         <v>14</v>
@@ -2168,13 +2571,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B16" t="s">
         <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D16">
         <v>15</v>
@@ -2182,13 +2585,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B17" t="s">
         <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D17">
         <v>16</v>
@@ -2202,7 +2605,7 @@
         <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -2210,13 +2613,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D19">
         <v>18</v>
@@ -2224,13 +2627,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C20" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D20">
         <v>19</v>
@@ -2238,10 +2641,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B21" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D21">
         <v>20</v>
@@ -2249,10 +2652,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D22">
         <v>21</v>
@@ -2260,10 +2663,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B23" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D23">
         <v>22</v>
@@ -2274,10 +2677,10 @@
         <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C24" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D24">
         <v>23</v>
@@ -2288,10 +2691,10 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="D25">
         <v>24</v>
@@ -2299,13 +2702,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B26" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C26" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D26">
         <v>25</v>
@@ -2313,13 +2716,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C27" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D27">
         <v>26</v>
@@ -2327,13 +2730,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B28" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C28" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D28">
         <v>27</v>
@@ -2341,13 +2744,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B29" t="s">
+        <v>163</v>
+      </c>
+      <c r="C29" t="s">
         <v>173</v>
-      </c>
-      <c r="C29" t="s">
-        <v>183</v>
       </c>
       <c r="D29">
         <v>28</v>
@@ -2355,13 +2758,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B30" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C30" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D30">
         <v>29</v>
@@ -2369,10 +2772,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B31" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D31">
         <v>30</v>
@@ -2380,13 +2783,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B32" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C32" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D32">
         <v>31</v>
@@ -2394,10 +2797,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B33" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D33">
         <v>32</v>
@@ -2405,13 +2808,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B34" t="s">
         <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D34">
         <v>33</v>
@@ -2419,13 +2822,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B35" t="s">
         <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D35">
         <v>34</v>
@@ -2433,13 +2836,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B36" t="s">
         <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D36">
         <v>35</v>
@@ -2447,13 +2850,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B37" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C37" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D37">
         <v>36</v>
@@ -2461,13 +2864,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B38" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C38" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D38">
         <v>37</v>
@@ -2481,7 +2884,7 @@
         <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="D39">
         <v>38</v>
@@ -2495,7 +2898,7 @@
         <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D40">
         <v>39</v>
@@ -2503,13 +2906,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B41" t="s">
         <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="D41">
         <v>40</v>
@@ -2517,13 +2920,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B42" t="s">
         <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="D42">
         <v>41</v>
@@ -2531,13 +2934,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B43" t="s">
         <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D43">
         <v>42</v>
@@ -2551,7 +2954,7 @@
         <v>55</v>
       </c>
       <c r="C44" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D44">
         <v>43</v>
@@ -2559,13 +2962,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B45" t="s">
         <v>50</v>
       </c>
       <c r="C45" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D45">
         <v>44</v>
@@ -2573,13 +2976,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B46" t="s">
         <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="D46">
         <v>45</v>
@@ -2587,13 +2990,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B47" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C47" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D47">
         <v>46</v>
@@ -2601,13 +3004,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B48" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C48" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="D48">
         <v>47</v>
@@ -2615,13 +3018,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B49" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C49" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="D49">
         <v>48</v>
@@ -2658,7 +3061,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2666,7 +3069,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -2698,7 +3101,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -2706,7 +3109,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -2714,7 +3117,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -2722,7 +3125,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -2746,7 +3149,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -2770,7 +3173,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -2783,11 +3186,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2825,25 +3228,102 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>390</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>416</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>417</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>394</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>72</v>
+        <v>395</v>
       </c>
       <c r="G2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B3" t="s">
+        <v>418</v>
+      </c>
+      <c r="C3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D3" t="s">
+        <v>419</v>
+      </c>
+      <c r="E3" t="s">
+        <v>378</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>364</v>
+      </c>
+      <c r="B4" t="s">
+        <v>420</v>
+      </c>
+      <c r="C4" t="s">
+        <v>421</v>
+      </c>
+      <c r="D4" t="s">
+        <v>422</v>
+      </c>
+      <c r="E4" t="s">
+        <v>369</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" t="s">
+        <v>423</v>
+      </c>
+      <c r="C5" t="s">
+        <v>424</v>
+      </c>
+      <c r="D5" t="s">
+        <v>425</v>
+      </c>
+      <c r="E5" t="s">
+        <v>290</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B6" t="s">
+        <v>426</v>
+      </c>
+      <c r="C6" t="s">
+        <v>427</v>
+      </c>
+      <c r="D6" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" t="s">
+        <v>306</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2853,11 +3333,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2875,16 +3355,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>64</v>
@@ -2893,16 +3373,16 @@
         <v>65</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>36</v>
@@ -2910,34 +3390,31 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>284</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>285</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>286</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>287</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>288</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>289</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" t="s">
-        <v>72</v>
+        <v>290</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>291</v>
       </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>267</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -2945,37 +3422,465 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>292</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>293</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>294</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>295</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>296</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>297</v>
       </c>
       <c r="G3" t="s">
-        <v>127</v>
-      </c>
-      <c r="H3" t="s">
-        <v>72</v>
+        <v>298</v>
       </c>
       <c r="I3" t="s">
-        <v>83</v>
+        <v>299</v>
       </c>
       <c r="J3" t="s">
-        <v>128</v>
+        <v>271</v>
       </c>
       <c r="K3">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D4" t="s">
+        <v>303</v>
+      </c>
+      <c r="E4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F4" t="s">
+        <v>305</v>
+      </c>
+      <c r="G4" t="s">
+        <v>306</v>
+      </c>
+      <c r="I4" t="s">
+        <v>307</v>
+      </c>
+      <c r="J4" t="s">
+        <v>308</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D5" t="s">
+        <v>312</v>
+      </c>
+      <c r="E5" t="s">
+        <v>313</v>
+      </c>
+      <c r="F5" t="s">
+        <v>314</v>
+      </c>
+      <c r="G5" t="s">
+        <v>315</v>
+      </c>
+      <c r="I5" t="s">
+        <v>316</v>
+      </c>
+      <c r="J5" t="s">
+        <v>317</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B6" t="s">
+        <v>319</v>
+      </c>
+      <c r="C6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D6" t="s">
+        <v>321</v>
+      </c>
+      <c r="E6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F6" t="s">
+        <v>323</v>
+      </c>
+      <c r="G6" t="s">
+        <v>324</v>
+      </c>
+      <c r="H6" t="s">
+        <v>325</v>
+      </c>
+      <c r="I6" t="s">
+        <v>326</v>
+      </c>
+      <c r="J6" t="s">
+        <v>327</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>328</v>
+      </c>
+      <c r="B7" t="s">
+        <v>329</v>
+      </c>
+      <c r="C7" t="s">
+        <v>330</v>
+      </c>
+      <c r="D7" t="s">
+        <v>331</v>
+      </c>
+      <c r="E7" t="s">
+        <v>332</v>
+      </c>
+      <c r="F7" t="s">
+        <v>333</v>
+      </c>
+      <c r="G7" t="s">
+        <v>334</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="I7" t="s">
+        <v>335</v>
+      </c>
+      <c r="J7" t="s">
+        <v>336</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>337</v>
+      </c>
+      <c r="B8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D8" t="s">
+        <v>340</v>
+      </c>
+      <c r="E8" t="s">
+        <v>341</v>
+      </c>
+      <c r="F8" t="s">
+        <v>342</v>
+      </c>
+      <c r="G8" t="s">
+        <v>343</v>
+      </c>
+      <c r="H8" t="s">
+        <v>344</v>
+      </c>
+      <c r="I8" t="s">
+        <v>345</v>
+      </c>
+      <c r="J8" t="s">
+        <v>346</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>347</v>
+      </c>
+      <c r="B9" t="s">
+        <v>348</v>
+      </c>
+      <c r="C9" t="s">
+        <v>349</v>
+      </c>
+      <c r="D9" t="s">
+        <v>350</v>
+      </c>
+      <c r="E9" t="s">
+        <v>351</v>
+      </c>
+      <c r="F9" t="s">
+        <v>352</v>
+      </c>
+      <c r="G9" t="s">
+        <v>353</v>
+      </c>
+      <c r="I9" t="s">
+        <v>354</v>
+      </c>
+      <c r="J9" t="s">
+        <v>355</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" t="s">
+        <v>356</v>
+      </c>
+      <c r="C10" t="s">
+        <v>357</v>
+      </c>
+      <c r="D10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E10" t="s">
+        <v>359</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>361</v>
+      </c>
+      <c r="J10" t="s">
+        <v>362</v>
+      </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>363</v>
+      </c>
+      <c r="B11" t="s">
+        <v>364</v>
+      </c>
+      <c r="C11" t="s">
+        <v>365</v>
+      </c>
+      <c r="D11" t="s">
+        <v>366</v>
+      </c>
+      <c r="E11" t="s">
+        <v>367</v>
+      </c>
+      <c r="F11" t="s">
+        <v>368</v>
+      </c>
+      <c r="G11" t="s">
+        <v>369</v>
+      </c>
+      <c r="I11" t="s">
+        <v>370</v>
+      </c>
+      <c r="J11" t="s">
+        <v>371</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>372</v>
+      </c>
+      <c r="B12" t="s">
+        <v>373</v>
+      </c>
+      <c r="C12" t="s">
+        <v>374</v>
+      </c>
+      <c r="D12" t="s">
+        <v>375</v>
+      </c>
+      <c r="E12" t="s">
+        <v>376</v>
+      </c>
+      <c r="F12" t="s">
+        <v>377</v>
+      </c>
+      <c r="G12" t="s">
+        <v>378</v>
+      </c>
+      <c r="I12" t="s">
+        <v>379</v>
+      </c>
+      <c r="J12" t="s">
+        <v>380</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>381</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>382</v>
+      </c>
+      <c r="D13" t="s">
+        <v>383</v>
+      </c>
+      <c r="E13" t="s">
+        <v>384</v>
+      </c>
+      <c r="F13" t="s">
+        <v>385</v>
+      </c>
+      <c r="G13" t="s">
+        <v>386</v>
+      </c>
+      <c r="I13" t="s">
+        <v>387</v>
+      </c>
+      <c r="J13" t="s">
+        <v>388</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>389</v>
+      </c>
+      <c r="B14" t="s">
+        <v>390</v>
+      </c>
+      <c r="C14" t="s">
+        <v>391</v>
+      </c>
+      <c r="D14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E14" t="s">
+        <v>393</v>
+      </c>
+      <c r="F14" t="s">
+        <v>394</v>
+      </c>
+      <c r="G14" t="s">
+        <v>395</v>
+      </c>
+      <c r="I14" t="s">
+        <v>396</v>
+      </c>
+      <c r="J14" t="s">
+        <v>397</v>
+      </c>
+      <c r="K14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>399</v>
+      </c>
+      <c r="B15" t="s">
+        <v>400</v>
+      </c>
+      <c r="C15" t="s">
+        <v>401</v>
+      </c>
+      <c r="D15" t="s">
+        <v>402</v>
+      </c>
+      <c r="E15" t="s">
+        <v>403</v>
+      </c>
+      <c r="F15" t="s">
+        <v>404</v>
+      </c>
+      <c r="G15" t="s">
+        <v>405</v>
+      </c>
+      <c r="H15" t="s">
+        <v>406</v>
+      </c>
+      <c r="I15" t="s">
+        <v>407</v>
+      </c>
+      <c r="J15" t="s">
+        <v>78</v>
+      </c>
+      <c r="K15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>408</v>
+      </c>
+      <c r="B16" t="s">
+        <v>409</v>
+      </c>
+      <c r="C16" t="s">
+        <v>410</v>
+      </c>
+      <c r="D16" t="s">
+        <v>411</v>
+      </c>
+      <c r="E16" t="s">
+        <v>412</v>
+      </c>
+      <c r="F16" t="s">
+        <v>413</v>
+      </c>
+      <c r="G16" t="s">
+        <v>414</v>
+      </c>
+      <c r="I16" t="s">
+        <v>415</v>
+      </c>
+      <c r="J16" t="s">
+        <v>267</v>
+      </c>
+      <c r="K16">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2988,7 +3893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
@@ -3006,22 +3911,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>36</v>
@@ -3029,22 +3934,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="E2" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="F2" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -3052,22 +3957,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B3" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="D3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="E3" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="F3" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -3075,22 +3980,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="B4" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="C4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" t="s">
         <v>254</v>
       </c>
-      <c r="D4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E4" t="s">
-        <v>264</v>
-      </c>
       <c r="F4" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -3098,22 +4003,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" t="s">
         <v>256</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>257</v>
-      </c>
-      <c r="D5" t="s">
-        <v>273</v>
-      </c>
-      <c r="E5" t="s">
-        <v>266</v>
-      </c>
-      <c r="F5" t="s">
-        <v>267</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -3121,22 +4026,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D6" t="s">
+        <v>262</v>
+      </c>
+      <c r="E6" t="s">
         <v>258</v>
       </c>
-      <c r="B6" t="s">
-        <v>250</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>259</v>
-      </c>
-      <c r="D6" t="s">
-        <v>272</v>
-      </c>
-      <c r="E6" t="s">
-        <v>268</v>
-      </c>
-      <c r="F6" t="s">
-        <v>269</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -3170,16 +4075,16 @@
         <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>36</v>
@@ -3187,19 +4092,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="E2" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3207,19 +4112,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C3" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D3" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="E3" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -3227,19 +4132,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B4" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E4" t="s">
         <v>281</v>
-      </c>
-      <c r="D4" t="s">
-        <v>282</v>
-      </c>
-      <c r="E4" t="s">
-        <v>291</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -3247,16 +4152,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="B5" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C5" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="E5" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -3264,16 +4169,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B6" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C6" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F6">
         <v>5</v>

</xml_diff>